<commit_message>
Replaced Incident number with Charge Identification, Added Citation number and Message Operation Code to Booking exchange
</commit_message>
<xml_diff>
--- a/schemas/BookingAndRelease_iepd/artifacts/Booking_MappingSpreadsheet_2025-05-13.xlsx
+++ b/schemas/BookingAndRelease_iepd/artifacts/Booking_MappingSpreadsheet_2025-05-13.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcp911gov-my.sharepoint.com/personal/jimpingel_missioncriticalpartners_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\BookingAndRelease_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{8D21533F-C88D-9B4F-B0E8-C0BFC9BF2C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA3C4C49-C6B4-42C3-A10E-3E8FBA25B579}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD8E340-5220-4C56-81A6-07106337FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29595" yWindow="300" windowWidth="27765" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21735" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Booking" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2266" uniqueCount="1080">
   <si>
     <t>Property Type</t>
   </si>
@@ -4337,6 +4337,27 @@
   </si>
   <si>
     <t>Delete every element other than nc:IdentificationID within scr:WarrantAugmentation/scr:WarrantIdentification</t>
+  </si>
+  <si>
+    <t>/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/j:ChargeInstrument/nc:DocumentIdentification/nc:IdenticationID</t>
+  </si>
+  <si>
+    <t>MessageOperationCode</t>
+  </si>
+  <si>
+    <t>A type of message operation.</t>
+  </si>
+  <si>
+    <t>nola-ext:UpdateCode</t>
+  </si>
+  <si>
+    <t>structures:MetadataType</t>
+  </si>
+  <si>
+    <t>/nola:BookingExchange/nola-ext:MessageUpdateCode</t>
+  </si>
+  <si>
+    <t>/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/j:ChargeIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -4444,7 +4465,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4482,6 +4503,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4590,7 +4617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4682,21 +4709,30 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5289,6 +5325,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5622,33 +5663,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B390143-938F-D746-8797-AAFFA7809748}">
-  <dimension ref="A1:R192"/>
+  <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="Q105" sqref="Q105:Q107"/>
+    <sheetView tabSelected="1" topLeftCell="F177" workbookViewId="0">
+      <selection activeCell="P193" sqref="P193"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="80.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="76.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.86328125" customWidth="1"/>
+    <col min="2" max="2" width="5.1328125" customWidth="1"/>
+    <col min="3" max="3" width="33.3984375" customWidth="1"/>
+    <col min="4" max="5" width="31.3984375" customWidth="1"/>
+    <col min="6" max="6" width="33.86328125" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" customWidth="1"/>
+    <col min="8" max="8" width="10.3984375" customWidth="1"/>
+    <col min="9" max="9" width="80.1328125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="76.3984375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.3984375" customWidth="1"/>
+    <col min="12" max="12" width="15.86328125" customWidth="1"/>
+    <col min="13" max="13" width="11.3984375" customWidth="1"/>
+    <col min="14" max="14" width="27.3984375" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" customWidth="1"/>
     <col min="16" max="16" width="56" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" ht="28.5">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5691,10 +5732,10 @@
       <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="41" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5732,7 +5773,7 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
     </row>
-    <row r="3" spans="1:16" s="37" customFormat="1">
+    <row r="3" spans="1:16" s="33" customFormat="1">
       <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
@@ -6878,7 +6919,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="38" customFormat="1">
+    <row r="30" spans="1:16" s="34" customFormat="1">
       <c r="A30" s="21" t="s">
         <v>3</v>
       </c>
@@ -6922,7 +6963,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="38" customFormat="1">
+    <row r="31" spans="1:16" s="34" customFormat="1">
       <c r="A31" s="21" t="s">
         <v>3</v>
       </c>
@@ -8258,7 +8299,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="64" spans="1:18" s="37" customFormat="1">
+    <row r="64" spans="1:18" s="33" customFormat="1" ht="28.5">
       <c r="A64" s="21" t="s">
         <v>3</v>
       </c>
@@ -8275,18 +8316,32 @@
       <c r="F64" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
+      <c r="G64" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>389</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="J64" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="K64" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="L64" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="M64" s="12"/>
       <c r="N64" s="12"/>
       <c r="O64" s="12"/>
-      <c r="P64" s="12"/>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="P64" s="40" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="28.5">
       <c r="A65" s="21" t="s">
         <v>3</v>
       </c>
@@ -8326,8 +8381,8 @@
       <c r="M65" s="12"/>
       <c r="N65" s="12"/>
       <c r="O65" s="12"/>
-      <c r="P65" s="12" t="s">
-        <v>392</v>
+      <c r="P65" s="40" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -9874,7 +9929,7 @@
       <c r="O104" s="11"/>
       <c r="P104" s="11"/>
     </row>
-    <row r="105" spans="1:16" s="37" customFormat="1">
+    <row r="105" spans="1:16" s="33" customFormat="1">
       <c r="A105" s="30" t="s">
         <v>3</v>
       </c>
@@ -9918,7 +9973,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="37" customFormat="1">
+    <row r="106" spans="1:16" s="33" customFormat="1">
       <c r="A106" s="16" t="s">
         <v>22</v>
       </c>
@@ -9956,7 +10011,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="107" spans="1:16" s="37" customFormat="1">
+    <row r="107" spans="1:16" s="33" customFormat="1">
       <c r="A107" s="21" t="s">
         <v>3</v>
       </c>
@@ -13050,7 +13105,7 @@
       <c r="O181" s="11"/>
       <c r="P181" s="11"/>
     </row>
-    <row r="182" spans="1:16" s="37" customFormat="1">
+    <row r="182" spans="1:16" s="33" customFormat="1">
       <c r="A182" s="17" t="s">
         <v>3</v>
       </c>
@@ -13096,7 +13151,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="183" spans="1:16" s="37" customFormat="1">
+    <row r="183" spans="1:16" s="33" customFormat="1">
       <c r="A183" s="16" t="s">
         <v>2</v>
       </c>
@@ -13126,7 +13181,7 @@
       <c r="O183" s="9"/>
       <c r="P183" s="9"/>
     </row>
-    <row r="184" spans="1:16" s="37" customFormat="1">
+    <row r="184" spans="1:16" s="33" customFormat="1">
       <c r="A184" s="16" t="s">
         <v>3</v>
       </c>
@@ -13164,7 +13219,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="185" spans="1:16" s="37" customFormat="1">
+    <row r="185" spans="1:16" s="33" customFormat="1">
       <c r="A185" s="16" t="s">
         <v>3</v>
       </c>
@@ -13204,7 +13259,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="186" spans="1:16" s="37" customFormat="1">
+    <row r="186" spans="1:16" s="33" customFormat="1">
       <c r="A186" s="16" t="s">
         <v>3</v>
       </c>
@@ -13244,7 +13299,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="187" spans="1:16" s="37" customFormat="1">
+    <row r="187" spans="1:16" s="33" customFormat="1">
       <c r="A187" s="16" t="s">
         <v>3</v>
       </c>
@@ -13284,7 +13339,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="188" spans="1:16" s="37" customFormat="1">
+    <row r="188" spans="1:16" s="33" customFormat="1">
       <c r="A188" s="16" t="s">
         <v>3</v>
       </c>
@@ -13324,7 +13379,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="189" spans="1:16" s="37" customFormat="1">
+    <row r="189" spans="1:16" s="33" customFormat="1">
       <c r="A189" s="16" t="s">
         <v>3</v>
       </c>
@@ -13364,7 +13419,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="190" spans="1:16" s="37" customFormat="1">
+    <row r="190" spans="1:16" s="33" customFormat="1">
       <c r="A190" s="16" t="s">
         <v>2</v>
       </c>
@@ -13388,7 +13443,7 @@
       <c r="O190" s="12"/>
       <c r="P190" s="9"/>
     </row>
-    <row r="191" spans="1:16" s="37" customFormat="1">
+    <row r="191" spans="1:16" s="33" customFormat="1">
       <c r="A191" s="16" t="s">
         <v>3</v>
       </c>
@@ -13426,8 +13481,8 @@
         <v>999</v>
       </c>
     </row>
-    <row r="192" spans="1:16" s="39" customFormat="1">
-      <c r="A192" s="16" t="s">
+    <row r="192" spans="1:16" s="35" customFormat="1">
+      <c r="A192" s="42" t="s">
         <v>3</v>
       </c>
       <c r="B192" s="9"/>
@@ -13462,6 +13517,44 @@
       <c r="O192" s="12"/>
       <c r="P192" s="9" t="s">
         <v>1005</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16" ht="15" customHeight="1">
+      <c r="A193" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193" s="9"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E193" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F193" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G193" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H193" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="I193" s="9"/>
+      <c r="J193" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="K193" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="L193" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M193" s="9"/>
+      <c r="N193" s="9"/>
+      <c r="O193" s="12"/>
+      <c r="P193" s="9" t="s">
+        <v>1078</v>
       </c>
     </row>
   </sheetData>
@@ -13478,13 +13571,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="178.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.3984375" customWidth="1"/>
+    <col min="2" max="2" width="178.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:2" ht="18">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>1006</v>
@@ -13499,7 +13592,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="37" t="s">
         <v>1009</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -13507,35 +13600,35 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="35"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="3" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="35"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="3" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="35"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="3" t="s">
         <v>1013</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="35"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="6" t="s">
         <v>1014</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="34"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="38" t="s">
         <v>1015</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -13543,17 +13636,17 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1">
-      <c r="A10" s="35"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="3" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="34"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="37" t="s">
         <v>247</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -13561,11 +13654,11 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="34"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="37" t="s">
         <v>255</v>
       </c>
       <c r="B14" s="28" t="s">
@@ -13573,23 +13666,23 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="35"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="28" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="35"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="28" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="35"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="28"/>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="37" t="s">
         <v>1021</v>
       </c>
       <c r="B18" s="28" t="s">
@@ -13597,11 +13690,11 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1">
-      <c r="A19" s="34"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="28"/>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="37" t="s">
         <v>1023</v>
       </c>
       <c r="B20" s="28" t="s">
@@ -13609,11 +13702,11 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
-      <c r="A21" s="34"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="28"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="37" t="s">
         <v>280</v>
       </c>
       <c r="B22" s="28" t="s">
@@ -13621,29 +13714,29 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="35"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="28" t="s">
         <v>1025</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="35"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="28" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="35"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="28" t="s">
         <v>1026</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="34"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="28"/>
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="37" t="s">
         <v>1027</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -13651,113 +13744,113 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="35"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="3" t="s">
         <v>1029</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1">
-      <c r="A29" s="35"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="3" t="s">
         <v>1030</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1">
-      <c r="A30" s="35"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="3" t="s">
         <v>1031</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1">
-      <c r="A31" s="35"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="3" t="s">
         <v>1032</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1">
-      <c r="A32" s="35"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="3" t="s">
         <v>1033</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1">
-      <c r="A33" s="35"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="3" t="s">
         <v>1034</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1">
-      <c r="A34" s="35"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="3" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1">
-      <c r="A35" s="35"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="3" t="s">
         <v>1036</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1">
-      <c r="A36" s="35"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="3" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1">
-      <c r="A37" s="35"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="3" t="s">
         <v>1038</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1">
-      <c r="A38" s="35"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="3" t="s">
         <v>1039</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" customHeight="1">
-      <c r="A39" s="35"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="3" t="s">
         <v>1040</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" customHeight="1">
-      <c r="A40" s="35"/>
+      <c r="A40" s="38"/>
       <c r="B40" s="3" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" customHeight="1">
-      <c r="A41" s="35"/>
+      <c r="A41" s="38"/>
       <c r="B41" s="3" t="s">
         <v>1028</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1">
-      <c r="A42" s="35"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="3" t="s">
         <v>1042</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" customHeight="1">
-      <c r="A43" s="35"/>
+      <c r="A43" s="38"/>
       <c r="B43" s="3" t="s">
         <v>1043</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1">
-      <c r="A44" s="35"/>
+      <c r="A44" s="38"/>
       <c r="B44" s="3" t="s">
         <v>1044</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="34"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="37" t="s">
         <v>136</v>
       </c>
       <c r="B46" s="28" t="s">
@@ -13765,77 +13858,77 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="35"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="28" t="s">
         <v>1045</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="35"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="28" t="s">
         <v>1046</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="35"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="3" t="s">
         <v>1047</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="35"/>
+      <c r="A50" s="38"/>
       <c r="B50" s="3" t="s">
         <v>1048</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="35"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="3" t="s">
         <v>1049</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="35"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="3" t="s">
         <v>1050</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="35"/>
+      <c r="A53" s="38"/>
       <c r="B53" s="3" t="s">
         <v>1051</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="35"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="3" t="s">
         <v>1052</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="35"/>
+      <c r="A55" s="38"/>
       <c r="B55" s="3" t="s">
         <v>1053</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="35"/>
+      <c r="A56" s="38"/>
       <c r="B56" s="3" t="s">
         <v>1054</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="35"/>
+      <c r="A57" s="38"/>
       <c r="B57" s="3" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="34"/>
+      <c r="A58" s="39"/>
       <c r="B58" s="28"/>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="37" t="s">
         <v>1056</v>
       </c>
       <c r="B59" s="28" t="s">
@@ -13843,23 +13936,23 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="35"/>
+      <c r="A60" s="38"/>
       <c r="B60" s="28" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="35"/>
+      <c r="A61" s="38"/>
       <c r="B61" s="28" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="34"/>
+      <c r="A62" s="39"/>
       <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="37" t="s">
         <v>1057</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -13867,29 +13960,29 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="35"/>
+      <c r="A64" s="38"/>
       <c r="B64" s="3" t="s">
         <v>1059</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="35"/>
+      <c r="A65" s="38"/>
       <c r="B65" s="28" t="s">
         <v>1060</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="30">
-      <c r="A66" s="35"/>
+    <row r="66" spans="1:2" ht="28.5">
+      <c r="A66" s="38"/>
       <c r="B66" s="28" t="s">
         <v>1061</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="34"/>
+      <c r="A67" s="39"/>
       <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="33" t="s">
+      <c r="A68" s="37" t="s">
         <v>1062</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -13897,43 +13990,43 @@
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="35"/>
+      <c r="A69" s="38"/>
       <c r="B69" s="3" t="s">
         <v>1064</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="35"/>
+      <c r="A70" s="38"/>
       <c r="B70" s="3" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="35"/>
+      <c r="A71" s="38"/>
       <c r="B71" s="3" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="35"/>
+      <c r="A72" s="38"/>
       <c r="B72" s="3" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="35"/>
+      <c r="A73" s="38"/>
       <c r="B73" s="28" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="35"/>
+      <c r="A74" s="38"/>
       <c r="B74" s="28" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="34"/>
+      <c r="A75" s="39"/>
       <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" ht="15" customHeight="1">
@@ -13956,6 +14049,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A76:A78"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A45"/>
@@ -13963,18 +14062,23 @@
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A63:A67"/>
     <mergeCell ref="A68:A75"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee7d25ce-443e-4f8a-a748-4259b6f1626e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="129c8279-1928-4e9e-bf04-a22cc9c6a884" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B27AFAFD56B51D40A0636D2EDDB429E9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13d31266acc58ebd7ba55a153b38d026">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="129c8279-1928-4e9e-bf04-a22cc9c6a884" xmlns:ns3="ee7d25ce-443e-4f8a-a748-4259b6f1626e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48ed0b125055c886dae4c0216e3655b5" ns2:_="" ns3:_="">
     <xsd:import namespace="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
@@ -14203,17 +14307,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee7d25ce-443e-4f8a-a748-4259b6f1626e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="129c8279-1928-4e9e-bf04-a22cc9c6a884" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14224,6 +14317,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{431E4146-98F3-4BF2-97B4-04BCB4BB8676}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee7d25ce-443e-4f8a-a748-4259b6f1626e"/>
+    <ds:schemaRef ds:uri="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A067CFA-EAD9-4768-BE86-4AE5F9AABE43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14242,17 +14346,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{431E4146-98F3-4BF2-97B4-04BCB4BB8676}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ee7d25ce-443e-4f8a-a748-4259b6f1626e"/>
-    <ds:schemaRef ds:uri="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4CC759A-AD2F-428D-BC04-038152F44D4B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed Replaced ChargeInstrument with nola-ext:ChargeAffidavit and added ChargeKey to Bond Update
</commit_message>
<xml_diff>
--- a/schemas/BookingAndRelease_iepd/artifacts/Booking_MappingSpreadsheet_2025-05-13.xlsx
+++ b/schemas/BookingAndRelease_iepd/artifacts/Booking_MappingSpreadsheet_2025-05-13.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\BookingAndRelease_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD8E340-5220-4C56-81A6-07106337FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5FA206-455E-42E0-818C-99C42EDFFE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21735" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4339,9 +4339,6 @@
     <t>Delete every element other than nc:IdentificationID within scr:WarrantAugmentation/scr:WarrantIdentification</t>
   </si>
   <si>
-    <t>/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/j:ChargeInstrument/nc:DocumentIdentification/nc:IdenticationID</t>
-  </si>
-  <si>
     <t>MessageOperationCode</t>
   </si>
   <si>
@@ -4358,6 +4355,9 @@
   </si>
   <si>
     <t>/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/j:ChargeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/nola:BookingExchange/j:Booking/j:Arrest/j:ArrestCharge[1]/nola-ext:ChargeAugmentation/nola-ext:ChargeAffidavitNumber</t>
   </si>
 </sst>
 </file>
@@ -4712,18 +4712,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4732,6 +4720,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5665,8 +5665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B390143-938F-D746-8797-AAFFA7809748}">
   <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F177" workbookViewId="0">
-      <selection activeCell="P193" sqref="P193"/>
+    <sheetView tabSelected="1" topLeftCell="F38" workbookViewId="0">
+      <selection activeCell="P64" sqref="P64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
@@ -5732,10 +5732,10 @@
       <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="37" t="s">
         <v>15</v>
       </c>
     </row>
@@ -8337,8 +8337,8 @@
       <c r="M64" s="12"/>
       <c r="N64" s="12"/>
       <c r="O64" s="12"/>
-      <c r="P64" s="40" t="s">
-        <v>1073</v>
+      <c r="P64" s="36" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="28.5">
@@ -8381,8 +8381,8 @@
       <c r="M65" s="12"/>
       <c r="N65" s="12"/>
       <c r="O65" s="12"/>
-      <c r="P65" s="40" t="s">
-        <v>1079</v>
+      <c r="P65" s="36" t="s">
+        <v>1078</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -13482,7 +13482,7 @@
       </c>
     </row>
     <row r="192" spans="1:16" s="35" customFormat="1">
-      <c r="A192" s="42" t="s">
+      <c r="A192" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B192" s="9"/>
@@ -13520,41 +13520,41 @@
       </c>
     </row>
     <row r="193" spans="1:16" ht="15" customHeight="1">
-      <c r="A193" s="42" t="s">
+      <c r="A193" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
       <c r="D193" s="9" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E193" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F193" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G193" s="9" t="s">
         <v>169</v>
       </c>
       <c r="H193" s="9" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="I193" s="9"/>
       <c r="J193" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="K193" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="L193" s="9" t="s">
         <v>1076</v>
-      </c>
-      <c r="K193" s="9" t="s">
-        <v>1076</v>
-      </c>
-      <c r="L193" s="9" t="s">
-        <v>1077</v>
       </c>
       <c r="M193" s="9"/>
       <c r="N193" s="9"/>
       <c r="O193" s="12"/>
       <c r="P193" s="9" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
   </sheetData>
@@ -13592,7 +13592,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1009</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -13600,35 +13600,35 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="38"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="3" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="38"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="3" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="38"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="3" t="s">
         <v>1013</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="38"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="6" t="s">
         <v>1014</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="41" t="s">
         <v>1015</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -13636,17 +13636,17 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1">
-      <c r="A10" s="38"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="3" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="39" t="s">
         <v>247</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -13654,11 +13654,11 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="39" t="s">
         <v>255</v>
       </c>
       <c r="B14" s="28" t="s">
@@ -13666,23 +13666,23 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="38"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="28" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="38"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="28" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="38"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="28"/>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="39" t="s">
         <v>1021</v>
       </c>
       <c r="B18" s="28" t="s">
@@ -13690,11 +13690,11 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1">
-      <c r="A19" s="39"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="28"/>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="39" t="s">
         <v>1023</v>
       </c>
       <c r="B20" s="28" t="s">
@@ -13702,11 +13702,11 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="28"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="39" t="s">
         <v>280</v>
       </c>
       <c r="B22" s="28" t="s">
@@ -13714,29 +13714,29 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="38"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="28" t="s">
         <v>1025</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="38"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="28" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="38"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="28" t="s">
         <v>1026</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="39"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="28"/>
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="39" t="s">
         <v>1027</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -13744,113 +13744,113 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1">
-      <c r="A28" s="38"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="3" t="s">
         <v>1029</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1">
-      <c r="A29" s="38"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="3" t="s">
         <v>1030</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1">
-      <c r="A30" s="38"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="3" t="s">
         <v>1031</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1">
-      <c r="A31" s="38"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="3" t="s">
         <v>1032</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1">
-      <c r="A32" s="38"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="3" t="s">
         <v>1033</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1">
-      <c r="A33" s="38"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="3" t="s">
         <v>1034</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1">
-      <c r="A34" s="38"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="3" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1">
-      <c r="A35" s="38"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="3" t="s">
         <v>1036</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" customHeight="1">
-      <c r="A36" s="38"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="3" t="s">
         <v>1037</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" customHeight="1">
-      <c r="A37" s="38"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="3" t="s">
         <v>1038</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1">
-      <c r="A38" s="38"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="3" t="s">
         <v>1039</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" customHeight="1">
-      <c r="A39" s="38"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="3" t="s">
         <v>1040</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" customHeight="1">
-      <c r="A40" s="38"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="3" t="s">
         <v>1041</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" customHeight="1">
-      <c r="A41" s="38"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="3" t="s">
         <v>1028</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1">
-      <c r="A42" s="38"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="3" t="s">
         <v>1042</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" customHeight="1">
-      <c r="A43" s="38"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="3" t="s">
         <v>1043</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" customHeight="1">
-      <c r="A44" s="38"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="3" t="s">
         <v>1044</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="39"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="3"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="39" t="s">
         <v>136</v>
       </c>
       <c r="B46" s="28" t="s">
@@ -13858,77 +13858,77 @@
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="38"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="28" t="s">
         <v>1045</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="38"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="28" t="s">
         <v>1046</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="38"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="3" t="s">
         <v>1047</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="38"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="3" t="s">
         <v>1048</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="38"/>
+      <c r="A51" s="41"/>
       <c r="B51" s="3" t="s">
         <v>1049</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="38"/>
+      <c r="A52" s="41"/>
       <c r="B52" s="3" t="s">
         <v>1050</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="38"/>
+      <c r="A53" s="41"/>
       <c r="B53" s="3" t="s">
         <v>1051</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="38"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="3" t="s">
         <v>1052</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="38"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="3" t="s">
         <v>1053</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="38"/>
+      <c r="A56" s="41"/>
       <c r="B56" s="3" t="s">
         <v>1054</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="38"/>
+      <c r="A57" s="41"/>
       <c r="B57" s="3" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="39"/>
+      <c r="A58" s="40"/>
       <c r="B58" s="28"/>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="39" t="s">
         <v>1056</v>
       </c>
       <c r="B59" s="28" t="s">
@@ -13936,23 +13936,23 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="38"/>
+      <c r="A60" s="41"/>
       <c r="B60" s="28" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="38"/>
+      <c r="A61" s="41"/>
       <c r="B61" s="28" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="39"/>
+      <c r="A62" s="40"/>
       <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="39" t="s">
         <v>1057</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -13960,29 +13960,29 @@
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="38"/>
+      <c r="A64" s="41"/>
       <c r="B64" s="3" t="s">
         <v>1059</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" s="38"/>
+      <c r="A65" s="41"/>
       <c r="B65" s="28" t="s">
         <v>1060</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="28.5">
-      <c r="A66" s="38"/>
+      <c r="A66" s="41"/>
       <c r="B66" s="28" t="s">
         <v>1061</v>
       </c>
     </row>
     <row r="67" spans="1:2">
-      <c r="A67" s="39"/>
+      <c r="A67" s="40"/>
       <c r="B67" s="5"/>
     </row>
     <row r="68" spans="1:2">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="39" t="s">
         <v>1062</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -13990,47 +13990,47 @@
       </c>
     </row>
     <row r="69" spans="1:2">
-      <c r="A69" s="38"/>
+      <c r="A69" s="41"/>
       <c r="B69" s="3" t="s">
         <v>1064</v>
       </c>
     </row>
     <row r="70" spans="1:2">
-      <c r="A70" s="38"/>
+      <c r="A70" s="41"/>
       <c r="B70" s="3" t="s">
         <v>1065</v>
       </c>
     </row>
     <row r="71" spans="1:2">
-      <c r="A71" s="38"/>
+      <c r="A71" s="41"/>
       <c r="B71" s="3" t="s">
         <v>1066</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="38"/>
+      <c r="A72" s="41"/>
       <c r="B72" s="3" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="73" spans="1:2">
-      <c r="A73" s="38"/>
+      <c r="A73" s="41"/>
       <c r="B73" s="28" t="s">
         <v>1068</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="38"/>
+      <c r="A74" s="41"/>
       <c r="B74" s="28" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="39"/>
+      <c r="A75" s="40"/>
       <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" ht="15" customHeight="1">
-      <c r="A76" s="36" t="s">
+      <c r="A76" s="42" t="s">
         <v>1070</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -14038,23 +14038,17 @@
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="36"/>
+      <c r="A77" s="42"/>
       <c r="B77" s="3" t="s">
         <v>1072</v>
       </c>
     </row>
     <row r="78" spans="1:2">
-      <c r="A78" s="36"/>
+      <c r="A78" s="42"/>
       <c r="B78" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A76:A78"/>
     <mergeCell ref="A22:A26"/>
     <mergeCell ref="A27:A45"/>
@@ -14062,6 +14056,12 @@
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A63:A67"/>
     <mergeCell ref="A68:A75"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14079,6 +14079,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B27AFAFD56B51D40A0636D2EDDB429E9" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13d31266acc58ebd7ba55a153b38d026">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="129c8279-1928-4e9e-bf04-a22cc9c6a884" xmlns:ns3="ee7d25ce-443e-4f8a-a748-4259b6f1626e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48ed0b125055c886dae4c0216e3655b5" ns2:_="" ns3:_="">
     <xsd:import namespace="129c8279-1928-4e9e-bf04-a22cc9c6a884"/>
@@ -14307,15 +14316,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{431E4146-98F3-4BF2-97B4-04BCB4BB8676}">
   <ds:schemaRefs>
@@ -14328,6 +14328,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4CC759A-AD2F-428D-BC04-038152F44D4B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A067CFA-EAD9-4768-BE86-4AE5F9AABE43}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14344,12 +14352,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4CC759A-AD2F-428D-BC04-038152F44D4B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>